<commit_message>
dari faris untuk kita semua
</commit_message>
<xml_diff>
--- a/app/Template.xlsx
+++ b/app/Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Kode</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Semester Ambil</t>
-  </si>
-  <si>
-    <t>Kurikulum</t>
   </si>
 </sst>
 </file>
@@ -357,10 +354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,7 +369,7 @@
     <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -385,9 +382,6 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>